<commit_message>
add validation filename ftp from config
</commit_message>
<xml_diff>
--- a/Traveloka_DataAutomation_Dispatcher_SFTP/Data/Config.xlsx
+++ b/Traveloka_DataAutomation_Dispatcher_SFTP/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John Suryajaya\Documents\UiPath\Traveloka_DataAutomation_Dispatcher_SFTP\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Documents\UiPath\Kalyana\Traveloka_DataAutomation_Dispatcher_SFTP\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F2839CF-9B88-45FE-9B39-34A90F1F57ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75520CE4-0346-4CE9-B9EC-5B77452E2707}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2581" yWindow="2581" windowWidth="19562" windowHeight="10230" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -181,28 +181,28 @@
     <t>PathSAKey</t>
   </si>
   <si>
+    <t>[Dev] RPA_Moon_FTP</t>
+  </si>
+  <si>
     <t>RPA_Moon_Cred_Gmail</t>
   </si>
   <si>
-    <t>RPA_Moon_PathMasterFolder</t>
-  </si>
-  <si>
-    <t>RPA_Moon_SheetIdConfig</t>
-  </si>
-  <si>
-    <t>RPA_Moon_PathMailTemplate</t>
-  </si>
-  <si>
-    <t>RPA_Moon_PathSaKey</t>
-  </si>
-  <si>
-    <t>RPA_Moon_FTP</t>
-  </si>
-  <si>
     <t>EmailSenderName</t>
   </si>
   <si>
     <t>RPA_Moon_SenderName</t>
+  </si>
+  <si>
+    <t>[DEV] RPA_Moon_SheetIdConfig</t>
+  </si>
+  <si>
+    <t>[DEV] RPA_Moon_PathMasterFolder</t>
+  </si>
+  <si>
+    <t>[DEV] RPA_Moon_PathMailTemplate</t>
+  </si>
+  <si>
+    <t>[DEV] RPA_Moon_PathSaKey</t>
   </si>
 </sst>
 </file>
@@ -583,7 +583,7 @@
   <dimension ref="A1:Z994"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A7" sqref="A7:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.375" defaultRowHeight="14.95" customHeight="1"/>
@@ -633,7 +633,7 @@
         <v>23</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>21</v>
@@ -671,7 +671,7 @@
         <v>45</v>
       </c>
       <c r="B7" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C7" t="s">
         <v>46</v>
@@ -2839,7 +2839,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.375" defaultRowHeight="14.95" customHeight="1"/>
@@ -2891,7 +2891,7 @@
         <v>48</v>
       </c>
       <c r="B2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.3" customHeight="1">
@@ -2899,7 +2899,7 @@
         <v>43</v>
       </c>
       <c r="B3" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.3" customHeight="1">
@@ -2907,7 +2907,7 @@
         <v>47</v>
       </c>
       <c r="B4" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.3" customHeight="1">
@@ -2915,15 +2915,15 @@
         <v>50</v>
       </c>
       <c r="B5" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.3" customHeight="1">
       <c r="A6" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B6" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.3" customHeight="1"/>

</xml_diff>